<commit_message>
updated multiple answers bug
</commit_message>
<xml_diff>
--- a/src/main/resources/questions.xlsx
+++ b/src/main/resources/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Coding Projects\Java\ultimate-spring-boot-exam\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482FF97-B0F7-4803-8D74-ED7B69509B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35455618-6867-4579-9468-377ADFE5328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{DD256250-6F2E-461F-A121-D4E0D938D1E6}"/>
   </bookViews>
@@ -6938,8 +6938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2E3107-8F71-44D1-A758-91CC0C525FFB}">
   <dimension ref="A1:J361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A360" workbookViewId="0">
-      <selection activeCell="H361" sqref="H361"/>
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
+      <selection activeCell="H302" sqref="H302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>